<commit_message>
Added config for password
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lovey\Automation\Assignment\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17160" windowHeight="2832"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Data_Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -471,7 +467,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>